<commit_message>
ezeket még át kell nézni
</commit_message>
<xml_diff>
--- a/JMDRGG_0316/1.feladat.xlsx
+++ b/JMDRGG_0316/1.feladat.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kill3\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://diakoffice-my.sharepoint.com/personal/rob__sulid_hu/Documents/EGYETEM/2020-2021-02/Operacios_rendszerek/gyakorlat/JMDRGGOsGyak/JMDRGG_0316/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{2B801397-BF7C-4608-805C-7E86354A09A3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="20" documentId="8_{2B801397-BF7C-4608-805C-7E86354A09A3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{5A8B3D45-8175-4596-A1EC-5603B812C22C}"/>
   <bookViews>
-    <workbookView xWindow="7665" yWindow="1800" windowWidth="17280" windowHeight="11385" xr2:uid="{310DC128-37BC-4D4D-8CEC-79966DB5066B}"/>
+    <workbookView xWindow="-120" yWindow="330" windowWidth="29040" windowHeight="15990" xr2:uid="{310DC128-37BC-4D4D-8CEC-79966DB5066B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -168,11 +168,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -490,20 +490,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0BC90CD2-480B-404C-898D-9E3B219B093B}">
   <dimension ref="A1:I36"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="E30" sqref="E30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="18.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="18.85546875" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="4"/>
-      <c r="C1" s="4"/>
-      <c r="D1" s="4"/>
-      <c r="E1" s="4"/>
+      <c r="B1" s="5"/>
+      <c r="C1" s="5"/>
+      <c r="D1" s="5"/>
+      <c r="E1" s="5"/>
       <c r="F1" s="2"/>
       <c r="G1" s="2"/>
       <c r="H1" s="2"/>
@@ -590,19 +593,19 @@
       <c r="A6" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="5">
+      <c r="B6" s="4">
         <f>B4+B5</f>
         <v>15</v>
       </c>
-      <c r="C6" s="5">
+      <c r="C6" s="4">
         <f t="shared" ref="C6:E6" si="0">C4+C5</f>
         <v>22</v>
       </c>
-      <c r="D6" s="5">
+      <c r="D6" s="4">
         <f t="shared" si="0"/>
         <v>48</v>
       </c>
-      <c r="E6" s="5">
+      <c r="E6" s="4">
         <f t="shared" si="0"/>
         <v>58</v>
       </c>
@@ -614,19 +617,19 @@
       <c r="A7" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B7" s="5">
+      <c r="B7" s="4">
         <f>B6 - B3 - B4</f>
         <v>0</v>
       </c>
-      <c r="C7" s="5">
+      <c r="C7" s="4">
         <f t="shared" ref="C7:E7" si="1">C6 - C3 - C4</f>
         <v>7</v>
       </c>
-      <c r="D7" s="5">
+      <c r="D7" s="4">
         <f t="shared" si="1"/>
         <v>10</v>
       </c>
-      <c r="E7" s="5">
+      <c r="E7" s="4">
         <f t="shared" si="1"/>
         <v>28</v>
       </c>
@@ -669,13 +672,13 @@
       <c r="H10" s="2"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" s="4" t="s">
+      <c r="A11" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="B11" s="4"/>
-      <c r="C11" s="4"/>
-      <c r="D11" s="4"/>
-      <c r="E11" s="4"/>
+      <c r="B11" s="5"/>
+      <c r="C11" s="5"/>
+      <c r="D11" s="5"/>
+      <c r="E11" s="5"/>
       <c r="F11" s="2"/>
       <c r="G11" s="2"/>
       <c r="H11" s="2"/>
@@ -742,16 +745,16 @@
       <c r="A15" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B15" s="5">
-        <v>0</v>
-      </c>
-      <c r="C15" s="5">
+      <c r="B15" s="4">
+        <v>0</v>
+      </c>
+      <c r="C15" s="4">
         <v>15</v>
       </c>
-      <c r="D15" s="5">
+      <c r="D15" s="4">
         <v>32</v>
       </c>
-      <c r="E15" s="5">
+      <c r="E15" s="4">
         <v>22</v>
       </c>
       <c r="F15" s="2"/>
@@ -762,17 +765,17 @@
       <c r="A16" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B16" s="5">
+      <c r="B16" s="4">
         <v>15</v>
       </c>
-      <c r="C16" s="5">
+      <c r="C16" s="4">
         <f>C15 + C14</f>
         <v>22</v>
       </c>
-      <c r="D16" s="5">
+      <c r="D16" s="4">
         <v>58</v>
       </c>
-      <c r="E16" s="5">
+      <c r="E16" s="4">
         <v>32</v>
       </c>
       <c r="F16" s="2"/>
@@ -783,16 +786,16 @@
       <c r="A17" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B17" s="5">
-        <v>0</v>
-      </c>
-      <c r="C17" s="5">
+      <c r="B17" s="4">
+        <v>0</v>
+      </c>
+      <c r="C17" s="4">
         <v>7</v>
       </c>
-      <c r="D17" s="5">
+      <c r="D17" s="4">
         <v>20</v>
       </c>
-      <c r="E17" s="5">
+      <c r="E17" s="4">
         <v>2</v>
       </c>
       <c r="F17" s="2"/>
@@ -902,13 +905,13 @@
       <c r="H24" s="2"/>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A25" s="4" t="s">
+      <c r="A25" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="B25" s="4"/>
-      <c r="C25" s="4"/>
-      <c r="D25" s="4"/>
-      <c r="E25" s="4"/>
+      <c r="B25" s="5"/>
+      <c r="C25" s="5"/>
+      <c r="D25" s="5"/>
+      <c r="E25" s="5"/>
       <c r="F25" s="3" t="s">
         <v>13</v>
       </c>
@@ -950,16 +953,16 @@
       <c r="C27" s="3">
         <v>15</v>
       </c>
-      <c r="D27" s="5">
-        <v>0</v>
-      </c>
-      <c r="E27" s="5">
+      <c r="D27" s="4">
+        <v>0</v>
+      </c>
+      <c r="E27" s="4">
         <v>10</v>
       </c>
-      <c r="F27" s="5">
-        <v>0</v>
-      </c>
-      <c r="G27" s="5">
+      <c r="F27" s="4">
+        <v>0</v>
+      </c>
+      <c r="G27" s="4">
         <v>5</v>
       </c>
       <c r="H27" s="3" t="s">
@@ -976,16 +979,16 @@
       <c r="C28" s="3">
         <v>7</v>
       </c>
-      <c r="D28" s="5">
+      <c r="D28" s="4">
         <v>10</v>
       </c>
-      <c r="E28" s="5">
+      <c r="E28" s="4">
         <v>17</v>
       </c>
-      <c r="F28" s="5">
+      <c r="F28" s="4">
         <v>2</v>
       </c>
-      <c r="G28" s="5">
+      <c r="G28" s="4">
         <v>0</v>
       </c>
       <c r="H28" s="3" t="s">
@@ -1002,16 +1005,16 @@
       <c r="C29" s="3">
         <v>4</v>
       </c>
-      <c r="D29" s="5">
+      <c r="D29" s="4">
         <v>17</v>
       </c>
-      <c r="E29" s="5">
+      <c r="E29" s="4">
         <v>21</v>
       </c>
-      <c r="F29" s="5">
+      <c r="F29" s="4">
         <v>7</v>
       </c>
-      <c r="G29" s="5">
+      <c r="G29" s="4">
         <v>0</v>
       </c>
       <c r="H29" s="3" t="s">
@@ -1028,18 +1031,14 @@
       <c r="C30" s="3">
         <v>26</v>
       </c>
-      <c r="D30" s="5">
+      <c r="D30" s="4">
         <v>21</v>
       </c>
-      <c r="E30" s="5">
-        <v>32</v>
-      </c>
-      <c r="F30" s="5">
+      <c r="E30" s="4"/>
+      <c r="F30" s="4">
         <v>9</v>
       </c>
-      <c r="G30" s="5">
-        <v>16</v>
-      </c>
+      <c r="G30" s="4"/>
       <c r="H30" s="3" t="s">
         <v>23</v>
       </c>
@@ -1054,18 +1053,10 @@
       <c r="C31" s="3">
         <v>10</v>
       </c>
-      <c r="D31" s="5">
-        <v>32</v>
-      </c>
-      <c r="E31" s="5">
-        <v>42</v>
-      </c>
-      <c r="F31" s="5">
-        <v>12</v>
-      </c>
-      <c r="G31" s="5">
-        <v>0</v>
-      </c>
+      <c r="D31" s="4"/>
+      <c r="E31" s="4"/>
+      <c r="F31" s="4"/>
+      <c r="G31" s="4"/>
       <c r="H31" s="3" t="s">
         <v>2</v>
       </c>
@@ -1080,18 +1071,10 @@
       <c r="C32" s="3">
         <v>16</v>
       </c>
-      <c r="D32" s="5">
-        <v>42</v>
-      </c>
-      <c r="E32" s="5">
-        <v>58</v>
-      </c>
-      <c r="F32" s="5">
-        <v>10</v>
-      </c>
-      <c r="G32" s="5">
-        <v>6</v>
-      </c>
+      <c r="D32" s="4"/>
+      <c r="E32" s="4"/>
+      <c r="F32" s="4"/>
+      <c r="G32" s="4"/>
       <c r="H32" s="3" t="s">
         <v>25</v>
       </c>
@@ -1106,18 +1089,10 @@
       <c r="C33" s="3">
         <v>6</v>
       </c>
-      <c r="D33" s="5">
-        <v>58</v>
-      </c>
-      <c r="E33" s="5">
-        <v>64</v>
-      </c>
-      <c r="F33" s="5">
-        <v>0</v>
-      </c>
-      <c r="G33" s="5">
-        <v>0</v>
-      </c>
+      <c r="D33" s="4"/>
+      <c r="E33" s="4"/>
+      <c r="F33" s="4"/>
+      <c r="G33" s="4"/>
       <c r="H33" s="3"/>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
@@ -1147,7 +1122,7 @@
       </c>
       <c r="C36" s="2">
         <f>SUM(F27:F33) /4</f>
-        <v>10</v>
+        <v>4.5</v>
       </c>
       <c r="E36" s="2"/>
       <c r="F36" s="2"/>

</xml_diff>

<commit_message>
round robin tabla at lett formalva
</commit_message>
<xml_diff>
--- a/JMDRGG_0316/1.feladat.xlsx
+++ b/JMDRGG_0316/1.feladat.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://diakoffice-my.sharepoint.com/personal/rob__sulid_hu/Documents/EGYETEM/2020-2021-02/Operacios_rendszerek/gyakorlat/JMDRGGOsGyak/JMDRGG_0316/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="20" documentId="8_{2B801397-BF7C-4608-805C-7E86354A09A3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{5A8B3D45-8175-4596-A1EC-5603B812C22C}"/>
+  <xr:revisionPtr revIDLastSave="93" documentId="8_{2B801397-BF7C-4608-805C-7E86354A09A3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{2F8E555C-1C58-4B6D-956C-59BA0B91E004}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="330" windowWidth="29040" windowHeight="15990" xr2:uid="{310DC128-37BC-4D4D-8CEC-79966DB5066B}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="26">
   <si>
     <t>P1</t>
   </si>
@@ -78,18 +78,9 @@
     <t>időszelet hossza : 10 (ms)</t>
   </si>
   <si>
-    <t>befejezés</t>
-  </si>
-  <si>
     <t>Várakozási idő</t>
   </si>
   <si>
-    <t>Maradék igény</t>
-  </si>
-  <si>
-    <t>Befejezéskor várakozó folyamatok</t>
-  </si>
-  <si>
     <t>P2, P1</t>
   </si>
   <si>
@@ -99,29 +90,35 @@
     <t>P1'</t>
   </si>
   <si>
-    <t>CPU idő (CPU igény)</t>
-  </si>
-  <si>
     <t>P3, P4</t>
   </si>
   <si>
     <t>P4, P3</t>
   </si>
   <si>
-    <t>p3'</t>
-  </si>
-  <si>
-    <t>p3</t>
-  </si>
-  <si>
     <t>P3''</t>
+  </si>
+  <si>
+    <t>CPU igény</t>
+  </si>
+  <si>
+    <t>Maradék cpu igény</t>
+  </si>
+  <si>
+    <t>Várakozó folyamatok</t>
+  </si>
+  <si>
+    <t>P3'</t>
+  </si>
+  <si>
+    <t>Átlagos várakozási idő:</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -132,6 +129,12 @@
     <font>
       <sz val="11"/>
       <color theme="4"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -157,7 +160,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -173,6 +176,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -490,8 +499,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0BC90CD2-480B-404C-898D-9E3B219B093B}">
   <dimension ref="A1:I36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="E30" sqref="E30"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="D37" sqref="D37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="18.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -500,13 +509,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="5"/>
-      <c r="C1" s="5"/>
-      <c r="D1" s="5"/>
-      <c r="E1" s="5"/>
+      <c r="B1" s="6"/>
+      <c r="C1" s="6"/>
+      <c r="D1" s="6"/>
+      <c r="E1" s="6"/>
       <c r="F1" s="2"/>
       <c r="G1" s="2"/>
       <c r="H1" s="2"/>
@@ -672,13 +681,13 @@
       <c r="H10" s="2"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" s="5" t="s">
+      <c r="A11" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="B11" s="5"/>
-      <c r="C11" s="5"/>
-      <c r="D11" s="5"/>
-      <c r="E11" s="5"/>
+      <c r="B11" s="6"/>
+      <c r="C11" s="6"/>
+      <c r="D11" s="6"/>
+      <c r="E11" s="6"/>
       <c r="F11" s="2"/>
       <c r="G11" s="2"/>
       <c r="H11" s="2"/>
@@ -908,191 +917,218 @@
       <c r="A25" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="B25" s="5"/>
+      <c r="B25" s="3" t="s">
+        <v>13</v>
+      </c>
       <c r="C25" s="5"/>
       <c r="D25" s="5"/>
       <c r="E25" s="5"/>
-      <c r="F25" s="3" t="s">
-        <v>13</v>
-      </c>
       <c r="G25" s="2"/>
       <c r="H25" s="2"/>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" s="2"/>
       <c r="B26" s="3" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>21</v>
+        <v>1</v>
       </c>
       <c r="D26" s="3" t="s">
-        <v>6</v>
+        <v>17</v>
       </c>
       <c r="E26" s="3" t="s">
-        <v>14</v>
+        <v>2</v>
       </c>
       <c r="F26" s="3" t="s">
-        <v>15</v>
+        <v>3</v>
       </c>
       <c r="G26" s="3" t="s">
-        <v>16</v>
+        <v>24</v>
       </c>
       <c r="H26" s="3" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="I26" s="1"/>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="B27" s="3">
         <v>0</v>
       </c>
       <c r="C27" s="3">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="D27" s="4">
-        <v>0</v>
-      </c>
-      <c r="E27" s="4">
         <v>10</v>
       </c>
-      <c r="F27" s="4">
-        <v>0</v>
+      <c r="E27" s="7">
+        <v>12</v>
+      </c>
+      <c r="F27" s="7">
+        <v>20</v>
       </c>
       <c r="G27" s="4">
-        <v>5</v>
-      </c>
-      <c r="H27" s="3" t="s">
-        <v>18</v>
+        <v>32</v>
+      </c>
+      <c r="H27" s="4">
+        <v>52</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
-        <v>1</v>
+        <v>21</v>
       </c>
       <c r="B28" s="3">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="C28" s="3">
         <v>7</v>
       </c>
       <c r="D28" s="4">
+        <v>5</v>
+      </c>
+      <c r="E28" s="7">
+        <v>26</v>
+      </c>
+      <c r="F28" s="7">
         <v>10</v>
       </c>
-      <c r="E28" s="4">
-        <v>17</v>
-      </c>
-      <c r="F28" s="4">
-        <v>2</v>
-      </c>
       <c r="G28" s="4">
-        <v>0</v>
-      </c>
-      <c r="H28" s="3" t="s">
-        <v>19</v>
+        <v>16</v>
+      </c>
+      <c r="H28" s="4">
+        <v>6</v>
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="B29" s="3">
+        <v>6</v>
+      </c>
+      <c r="B29" s="4">
+        <v>0</v>
+      </c>
+      <c r="C29" s="4">
         <v>10</v>
-      </c>
-      <c r="C29" s="3">
-        <v>4</v>
       </c>
       <c r="D29" s="4">
         <v>17</v>
       </c>
       <c r="E29" s="4">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="F29" s="4">
-        <v>7</v>
+        <v>32</v>
       </c>
       <c r="G29" s="4">
-        <v>0</v>
-      </c>
-      <c r="H29" s="3" t="s">
-        <v>22</v>
+        <v>42</v>
+      </c>
+      <c r="H29" s="4">
+        <v>52</v>
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B30" s="3">
-        <v>12</v>
-      </c>
-      <c r="C30" s="3">
-        <v>26</v>
+        <v>7</v>
+      </c>
+      <c r="B30" s="4">
+        <v>10</v>
+      </c>
+      <c r="C30" s="4">
+        <v>17</v>
       </c>
       <c r="D30" s="4">
-        <v>21</v>
-      </c>
-      <c r="E30" s="4"/>
+        <v>22</v>
+      </c>
+      <c r="E30" s="4">
+        <v>32</v>
+      </c>
       <c r="F30" s="4">
-        <v>9</v>
-      </c>
-      <c r="G30" s="4"/>
-      <c r="H30" s="3" t="s">
-        <v>23</v>
+        <v>42</v>
+      </c>
+      <c r="G30" s="4">
+        <v>52</v>
+      </c>
+      <c r="H30" s="4">
+        <v>58</v>
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B31" s="3">
-        <v>20</v>
-      </c>
-      <c r="C31" s="3">
+        <v>14</v>
+      </c>
+      <c r="B31" s="4">
+        <v>0</v>
+      </c>
+      <c r="C31" s="4">
+        <v>2</v>
+      </c>
+      <c r="D31" s="4">
+        <v>7</v>
+      </c>
+      <c r="E31" s="4">
         <v>10</v>
       </c>
-      <c r="D31" s="4"/>
-      <c r="E31" s="4"/>
-      <c r="F31" s="4"/>
-      <c r="G31" s="4"/>
-      <c r="H31" s="3" t="s">
-        <v>2</v>
+      <c r="F31" s="4">
+        <v>12</v>
+      </c>
+      <c r="G31" s="4">
+        <v>10</v>
+      </c>
+      <c r="H31" s="4">
+        <v>0</v>
       </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="B32" s="3">
-        <v>32</v>
-      </c>
-      <c r="C32" s="3">
+        <v>22</v>
+      </c>
+      <c r="B32" s="4">
+        <v>5</v>
+      </c>
+      <c r="C32" s="4">
+        <v>0</v>
+      </c>
+      <c r="D32" s="4">
+        <v>0</v>
+      </c>
+      <c r="E32" s="4">
         <v>16</v>
       </c>
-      <c r="D32" s="4"/>
-      <c r="E32" s="4"/>
-      <c r="F32" s="4"/>
-      <c r="G32" s="4"/>
-      <c r="H32" s="3" t="s">
-        <v>25</v>
+      <c r="F32" s="4">
+        <v>0</v>
+      </c>
+      <c r="G32" s="4">
+        <v>6</v>
+      </c>
+      <c r="H32" s="4">
+        <v>0</v>
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="B33" s="3">
-        <v>58</v>
-      </c>
-      <c r="C33" s="3">
-        <v>6</v>
-      </c>
-      <c r="D33" s="4"/>
-      <c r="E33" s="4"/>
-      <c r="F33" s="4"/>
-      <c r="G33" s="4"/>
+        <v>23</v>
+      </c>
+      <c r="B33" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C33" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="D33" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="E33" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="F33" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="G33" s="4" t="s">
+        <v>2</v>
+      </c>
       <c r="H33" s="3"/>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
@@ -1118,11 +1154,11 @@
     <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" s="2"/>
       <c r="B36" s="2" t="s">
-        <v>10</v>
+        <v>25</v>
       </c>
       <c r="C36" s="2">
-        <f>SUM(F27:F33) /4</f>
-        <v>4.5</v>
+        <f>SUM(B31:H31)/4</f>
+        <v>10.25</v>
       </c>
       <c r="E36" s="2"/>
       <c r="F36" s="2"/>
@@ -1130,10 +1166,9 @@
       <c r="H36" s="2"/>
     </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="2">
     <mergeCell ref="A1:E1"/>
     <mergeCell ref="A11:E11"/>
-    <mergeCell ref="A25:E25"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>